<commit_message>
order add area flag 1=大连 0=沈阳
</commit_message>
<xml_diff>
--- a/src/test/doc/shiro/客户权限测试账号.xlsx
+++ b/src/test/doc/shiro/客户权限测试账号.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="87">
   <si>
     <t>总经理</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,15 +249,6 @@
     <t>fzjl2</t>
   </si>
   <si>
-    <t>hygl</t>
-  </si>
-  <si>
-    <t>hycw</t>
-  </si>
-  <si>
-    <t>hykf</t>
-  </si>
-  <si>
     <t>hywjs</t>
   </si>
   <si>
@@ -271,9 +262,6 @@
   </si>
   <si>
     <t>jdzg2</t>
-  </si>
-  <si>
-    <t>scb</t>
   </si>
   <si>
     <t>htgl</t>
@@ -596,6 +584,22 @@
       <t xml:space="preserve">
 赠品明细统计</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hykf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hycw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hygl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1073,9 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1574,7 +1578,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>40</v>
@@ -1596,7 +1600,7 @@
     <row r="24" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
       <c r="C24" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>40</v>
@@ -1616,7 +1620,7 @@
     <row r="25" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
       <c r="C25" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>40</v>
@@ -1636,7 +1640,7 @@
     <row r="26" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
       <c r="C26" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>40</v>
@@ -1656,7 +1660,7 @@
     <row r="27" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>40</v>
@@ -1676,7 +1680,7 @@
     <row r="28" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
       <c r="C28" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>40</v>
@@ -1696,7 +1700,7 @@
     <row r="29" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B29" s="8"/>
       <c r="C29" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>40</v>
@@ -1716,7 +1720,7 @@
     <row r="30" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
       <c r="C30" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>40</v>
@@ -1736,7 +1740,7 @@
     <row r="31" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
       <c r="C31" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>40</v>
@@ -1756,7 +1760,7 @@
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
       <c r="C32" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>40</v>
@@ -1776,7 +1780,7 @@
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="8"/>
       <c r="C33" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>40</v>
@@ -1796,7 +1800,7 @@
     <row r="34" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
       <c r="C34" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>40</v>
@@ -1820,7 +1824,7 @@
     <row r="35" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
       <c r="C35" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>40</v>
@@ -1844,7 +1848,7 @@
     <row r="36" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
       <c r="C36" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>40</v>
@@ -1868,7 +1872,7 @@
     <row r="37" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
       <c r="C37" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>40</v>
@@ -1882,7 +1886,9 @@
       <c r="G37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2031,7 +2037,7 @@
         <v>50</v>
       </c>
       <c r="F46" s="11">
-        <v>123457</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
@@ -2042,7 +2048,7 @@
         <v>61</v>
       </c>
       <c r="F47" s="11">
-        <v>123458</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.3">
@@ -2050,10 +2056,10 @@
         <v>52</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F48" s="11">
-        <v>123459</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.3">
@@ -2061,10 +2067,10 @@
         <v>42</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F49" s="11">
-        <v>123460</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.3">
@@ -2072,10 +2078,10 @@
         <v>53</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F50" s="11">
-        <v>123461</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.3">
@@ -2083,10 +2089,10 @@
         <v>54</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F51" s="11">
-        <v>123462</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.3">
@@ -2094,10 +2100,10 @@
         <v>55</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F52" s="11">
-        <v>123463</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.3">
@@ -2105,10 +2111,10 @@
         <v>56</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F53" s="11">
-        <v>123464</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.3">
@@ -2116,10 +2122,10 @@
         <v>57</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F54" s="11">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.3">
@@ -2127,10 +2133,10 @@
         <v>58</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F55" s="11">
-        <v>123466</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.3">
@@ -2138,10 +2144,10 @@
         <v>59</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F56" s="11">
-        <v>123467</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.3">
@@ -2149,10 +2155,10 @@
         <v>60</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F57" s="11">
-        <v>123468</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>